<commit_message>
added plotting script for expriment
</commit_message>
<xml_diff>
--- a/PartC/Performance_testing/Perfmon_plots/Performance Counter.xlsx
+++ b/PartC/Performance_testing/Perfmon_plots/Performance Counter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwang\OneDrive\Desktop\MCGILL\FALL 2024\ECSE 429\Project\Part1\GitHub\ECSE429_Project\PartC\Performance_testing\Perfmon_plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{903F7ABF-3887-477C-957E-8A6D327063F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3841C24-926A-4B6A-B399-F31DBB869552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9A1770FA-FDC2-439F-BEFE-A6FB0FB04719}"/>
   </bookViews>
@@ -2563,16 +2563,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2599,15 +2599,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2956,7 +2956,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD22" sqref="AD22"/>
+      <selection activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>